<commit_message>
added cables to network
</commit_message>
<xml_diff>
--- a/Load List.xlsx
+++ b/Load List.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -53,7 +53,7 @@
     <t xml:space="preserve">name</t>
   </si>
   <si>
-    <t xml:space="preserve">_ohm_per_km</t>
+    <t xml:space="preserve">r_ohm_per_km</t>
   </si>
   <si>
     <t xml:space="preserve">x_ohm_per_km</t>
@@ -62,16 +62,13 @@
     <t xml:space="preserve">c_nf_per_km</t>
   </si>
   <si>
-    <t xml:space="preserve">type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">q_mm2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">alpha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cs</t>
+    <t xml:space="preserve">max_i_ka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CustomCable1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CustomCable2</t>
   </si>
 </sst>
 </file>
@@ -107,6 +104,7 @@
       <sz val="10"/>
       <name val="Courier New"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -151,7 +149,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -164,8 +162,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -293,8 +299,8 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -388,24 +394,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="13.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.81"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -417,19 +420,42 @@
       <c r="D1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="3" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="B2" s="5" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="C2" s="5" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>300</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E2" s="0" t="s">
-        <v>16</v>
+      <c r="B3" s="5" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>250</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>